<commit_message>
Stundensatz auf 80€ gesenkt (gemäß. Projektauftrag.md)
</commit_message>
<xml_diff>
--- a/Orga/Kostenrechnung.xlsx
+++ b/Orga/Kostenrechnung.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A211U09\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moshbit\source\repos\myTodo\Orga\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3E36D4-C289-4DD7-AC65-2B2F703F2EF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12615"/>
+    <workbookView xWindow="360" yWindow="0" windowWidth="17595" windowHeight="10455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
   </numFmts>
@@ -363,11 +364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,14 +378,14 @@
         <v>3</v>
       </c>
       <c r="E1" s="2">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2">
         <f>E1*8</f>
-        <v>960</v>
+        <v>640</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
@@ -407,7 +408,7 @@
       </c>
       <c r="D3" s="2">
         <f>C3*$H$1</f>
-        <v>2880</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -419,7 +420,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D15" si="0">C4*$H$1</f>
-        <v>1920</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -431,7 +432,7 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>2880</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -467,7 +468,7 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>2880</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -479,7 +480,7 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>2880</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -491,7 +492,7 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>2880</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -503,7 +504,7 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>2880</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -515,7 +516,7 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>2880</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -527,7 +528,7 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>1920</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -539,7 +540,7 @@
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>1920</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -551,7 +552,7 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>1920</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,7 +561,7 @@
       </c>
       <c r="D17" s="2">
         <f>SUM(D3:D15)</f>
-        <v>27840</v>
+        <v>18560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>